<commit_message>
simple out flight and undo out flight delete flight
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/GO_Course_Information.xlsx
+++ b/src/main/resources/input_excel_file/booking/GO_Course_Information.xlsx
@@ -4,12 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
-    <sheet name="Create_Flight_1Player" sheetId="1" r:id="rId1"/>
+    <sheet name="Create_Flight" sheetId="1" r:id="rId1"/>
     <sheet name="Out_All_Flight" sheetId="3" r:id="rId2"/>
-    <sheet name="Check_In_Ekyc" sheetId="2" r:id="rId3"/>
+    <sheet name="Simple_Out_Flight_Player1" sheetId="2" r:id="rId3"/>
+    <sheet name="Simple_Out_Flight_Player2" sheetId="7" r:id="rId4"/>
+    <sheet name="Simple_Out_Flight_Player3" sheetId="8" r:id="rId5"/>
+    <sheet name="Simple_Out_Flight_Player4" sheetId="9" r:id="rId6"/>
+    <sheet name="Undo_Out_Flight_Player1" sheetId="5" r:id="rId7"/>
+    <sheet name="Undo_Out_Flight_Player2" sheetId="10" r:id="rId8"/>
+    <sheet name="Undo_Out_Flight_Player3" sheetId="11" r:id="rId9"/>
+    <sheet name="Undo_Out_Flight_Player4" sheetId="12" r:id="rId10"/>
+    <sheet name="Delete_Attach_Flight_Player1" sheetId="4" r:id="rId11"/>
+    <sheet name="Delete_Attach_Flight_Player2" sheetId="13" r:id="rId12"/>
+    <sheet name="Delete_Attach_Flight_Player3" sheetId="14" r:id="rId13"/>
+    <sheet name="Delete_Attach_Flight_Player4" sheetId="15" r:id="rId14"/>
+    <sheet name="Add_Bag_To_Flight" sheetId="6" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="153">
   <si>
     <t>tc_id</t>
   </si>
@@ -262,9 +274,18 @@
     <t>{{CTX:BAG_2}}</t>
   </si>
   <si>
+    <t>05</t>
+  </si>
+  <si>
     <t>{{CTX:CUSTOMER_NAME_2}}</t>
   </si>
   <si>
+    <t>{{CTX:BAG_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:CUSTOMER_NAME_3}}</t>
+  </si>
+  <si>
     <t>Kiểm tra ghép xe 4 player + đi riêng xe</t>
   </si>
   <si>
@@ -274,6 +295,33 @@
     <t>Kiểm tra ghép xe 4 player + đi riêng xe + đặt caddie</t>
   </si>
   <si>
+    <t>CF_3_PLAYER_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra ghép xe 3 player</t>
+  </si>
+  <si>
+    <t>create_flight_3_player_request.json</t>
+  </si>
+  <si>
+    <t>CF_3_PLAYER_002</t>
+  </si>
+  <si>
+    <t>Kiểm tra ghép xe 3 player + đi riêng xe</t>
+  </si>
+  <si>
+    <t>CF_3_PLAYER_003</t>
+  </si>
+  <si>
+    <t>Kiểm tra ghép xe 3 player + đặt caddie</t>
+  </si>
+  <si>
+    <t>CF_3_PLAYER_004</t>
+  </si>
+  <si>
+    <t>Kiểm tra ghép xe 3 player + đi riêng xe + đặt caddie</t>
+  </si>
+  <si>
     <t>flight_id</t>
   </si>
   <si>
@@ -292,7 +340,7 @@
     <t>assert_message</t>
   </si>
   <si>
-    <t>Out_All_Flight_001</t>
+    <t>OUT_All_FLIGHT_001</t>
   </si>
   <si>
     <t>Kiểm tra out all flight 18 hole</t>
@@ -310,43 +358,148 @@
     <t>out_all_flight_expect.json</t>
   </si>
   <si>
-    <t>check_sum</t>
+    <t>bag</t>
+  </si>
+  <si>
+    <t>caddie_code</t>
+  </si>
+  <si>
+    <t>buggy_code</t>
+  </si>
+  <si>
+    <t>SIMPLE_OUT_FLIGHT_PLAYER1_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra simple all flight 18 hole khi ghép chung 1 flight</t>
+  </si>
+  <si>
+    <t>simple_out_flight_request.json</t>
+  </si>
+  <si>
+    <t>simple_out_flight_expect.json</t>
+  </si>
+  <si>
+    <t>SIMPLE_OUT_FLIGHT_PLAYER2_001</t>
+  </si>
+  <si>
+    <t>SIMPLE_OUT_FLIGHT_PLAYER3_001</t>
+  </si>
+  <si>
+    <t>SIMPLE_OUT_FLIGHT_PLAYER4_001</t>
+  </si>
+  <si>
+    <t>UNDO_OUT_FLIGHT_PLAYER1_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra undo out flight cho player 1 khi ghép chung 1 flight</t>
+  </si>
+  <si>
+    <t>undo_out_flight_request.json</t>
+  </si>
+  <si>
+    <t>undo_out_flight_expect.json</t>
+  </si>
+  <si>
+    <t>UNDO_OUT_FLIGHT_PLAYER2_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra undo out flight cho player 2 khi ghép chung 1 flight</t>
+  </si>
+  <si>
+    <t>UNDO_OUT_FLIGHT_PLAYER3_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra undo out flight cho player 3 khi ghép chung 1 flight</t>
+  </si>
+  <si>
+    <t>UNDO_OUT_FLIGHT_PLAYER4_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra undo out flight cho player 4 khi ghép chung 1 flight</t>
   </si>
   <si>
     <t>booking_uid</t>
   </si>
   <si>
-    <t>assert_code</t>
-  </si>
-  <si>
-    <t>assert_desc</t>
-  </si>
-  <si>
-    <t>CI_EKYC_001</t>
-  </si>
-  <si>
-    <t>MB_Kiểm tra check in bag</t>
-  </si>
-  <si>
-    <t>check_in_ekyc_request.json</t>
-  </si>
-  <si>
-    <t>{{CHECKSUM}}</t>
+    <t>note</t>
+  </si>
+  <si>
+    <t>is_out_caddie</t>
+  </si>
+  <si>
+    <t>is_out_buggy</t>
+  </si>
+  <si>
+    <t>assert_added_flight</t>
+  </si>
+  <si>
+    <t>assert_bag_status</t>
+  </si>
+  <si>
+    <t>assert_flight_id</t>
+  </si>
+  <si>
+    <t>DELETE_ATTACH_FLIGHT_PLAYER1_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra xóa flight cho player 1</t>
+  </si>
+  <si>
+    <t>delete_attach_flight_request.json</t>
   </si>
   <si>
     <t>{{CTX:BOOKING_UID_0}}</t>
   </si>
   <si>
+    <t>delete_attach_flight_expect.json</t>
+  </si>
+  <si>
+    <t>WAITING</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>DELETE_ATTACH_FLIGHT_PLAYER2_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra xóa flight cho player 2</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_UID_1}}</t>
+  </si>
+  <si>
+    <t>DELETE_ATTACH_FLIGHT_PLAYER3_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra xóa flight cho player 3</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_UID_2}}</t>
+  </si>
+  <si>
+    <t>DELETE_ATTACH_FLIGHT_PLAYER4_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra xóa flight cho player 4</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_UID_3}}</t>
+  </si>
+  <si>
+    <t>ADD_BAG_TO_FLIGHT_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra add bag to flight khi ghép chung 1 flight</t>
+  </si>
+  <si>
+    <t>add_bag_to_flight_request.json</t>
+  </si>
+  <si>
     <t>{{TODAY}}</t>
   </si>
   <si>
-    <t>check_in_ekyc_expect.json</t>
-  </si>
-  <si>
-    <t>00</t>
-  </si>
-  <si>
-    <t>Success</t>
+    <t>add_bag_to_flight_expect.json</t>
   </si>
 </sst>
 </file>
@@ -359,7 +512,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +540,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -548,13 +709,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -892,137 +1053,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1032,49 +1193,67 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1083,13 +1262,10 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1628,10 +1804,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AO13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AK19" sqref="AK19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="A6" sqref="$A6:$XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -1644,13 +1820,13 @@
     <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
     <col min="7" max="7" width="31.8571428571429" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.7142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.8380952380952" style="12" customWidth="1"/>
-    <col min="10" max="10" width="21.5714285714286" style="12" customWidth="1"/>
+    <col min="9" max="9" width="17.8380952380952" style="11" customWidth="1"/>
+    <col min="10" max="10" width="21.5714285714286" style="11" customWidth="1"/>
     <col min="11" max="11" width="21.4285714285714" style="1" customWidth="1"/>
     <col min="12" max="12" width="28.7142857142857" style="1" customWidth="1"/>
-    <col min="13" max="14" width="17.8380952380952" style="12" customWidth="1"/>
+    <col min="13" max="14" width="17.8380952380952" style="11" customWidth="1"/>
     <col min="15" max="37" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="38" max="38" width="17.8380952380952" style="12" customWidth="1"/>
+    <col min="38" max="38" width="17.8380952380952" style="11" customWidth="1"/>
     <col min="39" max="39" width="35.5714285714286" style="1" customWidth="1"/>
     <col min="40" max="40" width="15.2857142857143" style="1" customWidth="1"/>
     <col min="41" max="41" width="20.8571428571429" style="1" customWidth="1"/>
@@ -1674,106 +1850,106 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="U1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="W1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="X1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Y1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AA1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="17" t="s">
+      <c r="AB1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AD1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AE1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AG1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AH1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AI1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="13" t="s">
+      <c r="AJ1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="13" t="s">
+      <c r="AK1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AL1" s="20" t="s">
         <v>37</v>
       </c>
       <c r="AM1" s="8" t="s">
@@ -1799,70 +1975,70 @@
       <c r="D2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16"/>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16" t="s">
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AK2" s="21" t="s">
+      <c r="AK2" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AL2" s="16" t="s">
+      <c r="AL2" s="22" t="s">
         <v>55</v>
       </c>
       <c r="AM2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AN2" s="7">
+      <c r="AN2" s="10">
         <v>200</v>
       </c>
       <c r="AO2" s="22" t="s">
@@ -1882,70 +2058,70 @@
       <c r="D3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="16"/>
-      <c r="AB3" s="16"/>
-      <c r="AC3" s="16"/>
-      <c r="AD3" s="16"/>
-      <c r="AE3" s="16"/>
-      <c r="AF3" s="16"/>
-      <c r="AG3" s="16"/>
-      <c r="AH3" s="16"/>
-      <c r="AI3" s="16"/>
-      <c r="AJ3" s="16" t="s">
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AJ3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AK3" s="21" t="s">
+      <c r="AK3" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="16" t="s">
+      <c r="AL3" s="22" t="s">
         <v>55</v>
       </c>
       <c r="AM3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AN3" s="7">
+      <c r="AN3" s="10">
         <v>200</v>
       </c>
       <c r="AO3" s="22" t="s">
@@ -1965,70 +2141,70 @@
       <c r="D4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16" t="s">
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AK4" s="21" t="s">
+      <c r="AK4" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AL4" s="16" t="s">
+      <c r="AL4" s="22" t="s">
         <v>55</v>
       </c>
       <c r="AM4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AN4" s="7">
+      <c r="AN4" s="10">
         <v>200</v>
       </c>
       <c r="AO4" s="22" t="s">
@@ -2048,70 +2224,70 @@
       <c r="D5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="16"/>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="16" t="s">
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="22"/>
+      <c r="AH5" s="22"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AK5" s="21" t="s">
+      <c r="AK5" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AL5" s="16" t="s">
+      <c r="AL5" s="22" t="s">
         <v>55</v>
       </c>
       <c r="AM5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AN5" s="7">
+      <c r="AN5" s="10">
         <v>200</v>
       </c>
       <c r="AO5" s="22" t="s">
@@ -2131,112 +2307,112 @@
       <c r="D6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="P6" s="20" t="s">
+      <c r="P6" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="Q6" s="20" t="s">
+      <c r="Q6" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="R6" s="16" t="s">
+      <c r="R6" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="S6" s="16" t="s">
+      <c r="S6" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="T6" s="20" t="s">
+      <c r="T6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="U6" s="20" t="s">
+      <c r="U6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="V6" s="7" t="s">
+      <c r="V6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="X6" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y6" s="16" t="s">
+      <c r="W6" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="X6" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="Z6" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA6" s="20" t="s">
+      <c r="Z6" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AB6" s="20" t="s">
+      <c r="AB6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AC6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD6" s="20" t="s">
+      <c r="AC6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD6" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="AE6" s="20" t="s">
+      <c r="AE6" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="AF6" s="16" t="s">
+      <c r="AF6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AG6" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH6" s="20" t="s">
+      <c r="AG6" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AI6" s="20" t="s">
+      <c r="AI6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AJ6" s="16" t="s">
+      <c r="AJ6" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AK6" s="21" t="s">
+      <c r="AK6" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AL6" s="16" t="s">
+      <c r="AL6" s="22" t="s">
         <v>55</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AN6" s="7">
+      <c r="AN6" s="10">
         <v>200</v>
       </c>
       <c r="AO6" s="22" t="s">
@@ -2248,7 +2424,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>43</v>
@@ -2256,112 +2432,112 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="L7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="P7" s="20" t="s">
+      <c r="P7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="Q7" s="20" t="s">
+      <c r="Q7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="R7" s="16" t="s">
+      <c r="R7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="16" t="s">
+      <c r="S7" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="T7" s="20" t="s">
+      <c r="T7" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="U7" s="20" t="s">
+      <c r="U7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="V7" s="7" t="s">
+      <c r="V7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="W7" s="20" t="s">
+      <c r="W7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="X7" s="20" t="s">
+      <c r="X7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="Y7" s="16" t="s">
+      <c r="Y7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="Z7" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA7" s="20" t="s">
+      <c r="Z7" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA7" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AB7" s="20" t="s">
+      <c r="AB7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AC7" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD7" s="20" t="s">
+      <c r="AC7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="AE7" s="20" t="s">
+      <c r="AE7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="AF7" s="16" t="s">
+      <c r="AF7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AG7" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH7" s="20" t="s">
+      <c r="AG7" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH7" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AI7" s="20" t="s">
+      <c r="AI7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AJ7" s="16" t="s">
+      <c r="AJ7" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AK7" s="21" t="s">
+      <c r="AK7" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AL7" s="16" t="s">
+      <c r="AL7" s="22" t="s">
         <v>55</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AN7" s="7">
+      <c r="AN7" s="10">
         <v>200</v>
       </c>
       <c r="AO7" s="22" t="s">
@@ -2373,7 +2549,7 @@
         <v>71</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>43</v>
@@ -2381,112 +2557,112 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="L8" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="N8" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="Q8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="R8" s="16" t="s">
+      <c r="R8" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="S8" s="16" t="s">
+      <c r="S8" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="U8" s="20" t="s">
+      <c r="U8" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="V8" s="7" t="s">
+      <c r="V8" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="W8" s="20" t="s">
+      <c r="W8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="X8" s="20" t="s">
+      <c r="X8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="Y8" s="16" t="s">
+      <c r="Y8" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="Z8" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA8" s="20" t="s">
+      <c r="Z8" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AB8" s="20" t="s">
+      <c r="AB8" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AC8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD8" s="20" t="s">
+      <c r="AC8" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="AE8" s="20" t="s">
+      <c r="AE8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="AF8" s="16" t="s">
+      <c r="AF8" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="AG8" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH8" s="20" t="s">
+      <c r="AG8" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AI8" s="20" t="s">
+      <c r="AI8" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AJ8" s="16" t="s">
+      <c r="AJ8" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AK8" s="21" t="s">
+      <c r="AK8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AL8" s="16" t="s">
+      <c r="AL8" s="22" t="s">
         <v>55</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AN8" s="7">
+      <c r="AN8" s="10">
         <v>200</v>
       </c>
       <c r="AO8" s="22" t="s">
@@ -2498,7 +2674,7 @@
         <v>71</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>43</v>
@@ -2506,115 +2682,1219 @@
       <c r="D9" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M9" s="20" t="s">
+      <c r="M9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="N9" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="O9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="P9" s="20" t="s">
+      <c r="P9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="Q9" s="20" t="s">
+      <c r="Q9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="R9" s="16" t="s">
+      <c r="R9" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="S9" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="T9" s="20" t="s">
+      <c r="T9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="20" t="s">
+      <c r="U9" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="V9" s="7" t="s">
+      <c r="V9" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="W9" s="20" t="s">
+      <c r="W9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="X9" s="20" t="s">
+      <c r="X9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="Y9" s="16" t="s">
+      <c r="Y9" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="Z9" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA9" s="20" t="s">
+      <c r="Z9" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AB9" s="20" t="s">
+      <c r="AB9" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AC9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD9" s="20" t="s">
+      <c r="AC9" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="AE9" s="20" t="s">
+      <c r="AE9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="AF9" s="16" t="s">
+      <c r="AF9" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AG9" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH9" s="20" t="s">
+      <c r="AG9" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AI9" s="20" t="s">
+      <c r="AI9" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AJ9" s="16" t="s">
+      <c r="AJ9" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AK9" s="21" t="s">
+      <c r="AK9" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AL9" s="16" t="s">
+      <c r="AL9" s="22" t="s">
         <v>55</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AN9" s="7">
+      <c r="AN9" s="10">
         <v>200</v>
       </c>
       <c r="AO9" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:41">
+      <c r="A10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P10" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q10" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="S10" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="W10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="X10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z10" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="26"/>
+      <c r="AJ10" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK10" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL10" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN10" s="10">
+        <v>200</v>
+      </c>
+      <c r="AO10" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:41">
+      <c r="A11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="S11" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="T11" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="U11" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="V11" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="W11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="X11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y11" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z11" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA11" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB11" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="26"/>
+      <c r="AE11" s="26"/>
+      <c r="AF11" s="22"/>
+      <c r="AG11" s="22"/>
+      <c r="AH11" s="26"/>
+      <c r="AI11" s="26"/>
+      <c r="AJ11" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK11" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL11" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN11" s="10">
+        <v>200</v>
+      </c>
+      <c r="AO11" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:41">
+      <c r="A12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="M12" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="R12" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="S12" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="T12" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="U12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="W12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="X12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y12" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z12" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA12" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="26"/>
+      <c r="AF12" s="22"/>
+      <c r="AG12" s="22"/>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK12" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL12" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN12" s="10">
+        <v>200</v>
+      </c>
+      <c r="AO12" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:41">
+      <c r="A13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P13" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q13" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="R13" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="S13" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="T13" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="U13" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="V13" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="W13" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="X13" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y13" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z13" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA13" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB13" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="26"/>
+      <c r="AE13" s="26"/>
+      <c r="AF13" s="22"/>
+      <c r="AG13" s="22"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26"/>
+      <c r="AJ13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK13" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL13" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN13" s="10">
+        <v>200</v>
+      </c>
+      <c r="AO13" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="31" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.2857142857143" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.2857142857143" style="11" customWidth="1"/>
+    <col min="10" max="10" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" ht="59" customHeight="1" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="10">
+        <v>200</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="33.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.8571428571429" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2857142857143" style="11" customWidth="1"/>
+    <col min="12" max="12" width="20.5714285714286" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
+      <c r="A2" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="10">
+        <v>200</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="33.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.8571428571429" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2857142857143" style="11" customWidth="1"/>
+    <col min="12" max="12" width="20.5714285714286" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
+      <c r="A2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="10">
+        <v>200</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="33.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.8571428571429" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2857142857143" style="11" customWidth="1"/>
+    <col min="12" max="12" width="20.5714285714286" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
+      <c r="A2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="10">
+        <v>200</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="33.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.8571428571429" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2857142857143" style="11" customWidth="1"/>
+    <col min="12" max="12" width="20.5714285714286" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
+      <c r="A2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="10">
+        <v>200</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="26.5714285714286" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.4285714285714" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="10" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.2857142857143" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.14285714285714" style="1"/>
+    <col min="14" max="14" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A2" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="10">
+        <v>200</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2630,12 +3910,12 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="13.7142857142857" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
@@ -2667,20 +3947,20 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>85</v>
+      <c r="E1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>38</v>
@@ -2689,44 +3969,44 @@
         <v>39</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A2" s="4" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="11">
+        <v>101</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="18">
         <v>18</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="18">
         <v>18</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="18">
         <v>18</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>91</v>
+      <c r="I2" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="7">
+        <v>104</v>
+      </c>
+      <c r="K2" s="10">
         <v>200</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="10" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2739,33 +4019,34 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="13.7142857142857" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.4285714285714" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.8571428571429" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7142857142857" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7142857142857" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.2857142857143" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.14285714285714" style="1"/>
+    <col min="17" max="17" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2782,69 +4063,722 @@
         <v>93</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>96</v>
+      <c r="O1" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A2" s="4" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>99</v>
+        <v>110</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7">
+        <v>18</v>
+      </c>
+      <c r="I2" s="7">
+        <v>18</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="10">
+        <v>200</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7142857142857" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.2857142857143" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.14285714285714" style="1"/>
+    <col min="17" max="17" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:15">
+      <c r="A2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="7">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7">
+        <v>18</v>
+      </c>
+      <c r="I2" s="7">
+        <v>18</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="10">
+        <v>200</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7142857142857" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.2857142857143" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.14285714285714" style="1"/>
+    <col min="17" max="17" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:15">
+      <c r="A2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="7">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7">
+        <v>18</v>
+      </c>
+      <c r="I2" s="7">
+        <v>18</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="10">
+        <v>200</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7142857142857" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.2857142857143" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.14285714285714" style="1"/>
+    <col min="17" max="17" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:15">
+      <c r="A2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="7">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7">
+        <v>18</v>
+      </c>
+      <c r="I2" s="7">
+        <v>18</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="10">
+        <v>200</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="34.5714285714286" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.2857142857143" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.2857142857143" style="11" customWidth="1"/>
+    <col min="10" max="10" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="59" customHeight="1" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="K2" s="7">
+      <c r="F2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="10">
         <v>200</v>
       </c>
-      <c r="L2" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="M2" s="7" t="s">
+      <c r="I2" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="36.1428571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.2857142857143" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.2857142857143" style="11" customWidth="1"/>
+    <col min="10" max="10" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>105</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" ht="59" customHeight="1" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="10">
+        <v>200</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="41" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.2857142857143" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.2857142857143" style="11" customWidth="1"/>
+    <col min="10" max="10" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" ht="59" customHeight="1" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="10">
+        <v>200</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add mini bar and driving
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/GO_Course_Information.xlsx
+++ b/src/main/resources/input_excel_file/booking/GO_Course_Information.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="10" activeTab="15"/>
+    <workbookView windowWidth="30240" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="Create_Flight" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="176">
   <si>
     <t>tc_id</t>
   </si>
@@ -275,34 +275,34 @@
     <t>{{CTX:BAG_2}}</t>
   </si>
   <si>
+    <t>{{CTX:CUSTOMER_NAME_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:BAG_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:CUSTOMER_NAME_3}}</t>
+  </si>
+  <si>
+    <t>Kiểm tra ghép xe 4 player + đi riêng xe</t>
+  </si>
+  <si>
+    <t>Kiểm tra ghép xe 4 player + đặt caddie</t>
+  </si>
+  <si>
+    <t>Kiểm tra ghép xe 4 player + đi riêng xe + đặt caddie</t>
+  </si>
+  <si>
+    <t>CF_3_PLAYER_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra ghép xe 3 player</t>
+  </si>
+  <si>
+    <t>create_flight_3_player_request.json</t>
+  </si>
+  <si>
     <t>05</t>
-  </si>
-  <si>
-    <t>{{CTX:CUSTOMER_NAME_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:BAG_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:CUSTOMER_NAME_3}}</t>
-  </si>
-  <si>
-    <t>Kiểm tra ghép xe 4 player + đi riêng xe</t>
-  </si>
-  <si>
-    <t>Kiểm tra ghép xe 4 player + đặt caddie</t>
-  </si>
-  <si>
-    <t>Kiểm tra ghép xe 4 player + đi riêng xe + đặt caddie</t>
-  </si>
-  <si>
-    <t>CF_3_PLAYER_001</t>
-  </si>
-  <si>
-    <t>Kiểm tra ghép xe 3 player</t>
-  </si>
-  <si>
-    <t>create_flight_3_player_request.json</t>
   </si>
   <si>
     <t>CF_3_PLAYER_002</t>
@@ -577,10 +577,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -598,18 +598,18 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
     </font>
     <font>
       <i/>
@@ -1111,16 +1111,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1253,7 +1253,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1263,17 +1263,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1281,19 +1281,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1302,32 +1296,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1343,7 +1337,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1870,35 +1864,35 @@
   <sheetPr/>
   <dimension ref="A1:AO13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="A6" sqref="$A6:$XFD6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.3142857142857" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.8571428571429" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.3125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.859375" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.8571428571429" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.8380952380952" style="12" customWidth="1"/>
-    <col min="10" max="10" width="21.5714285714286" style="12" customWidth="1"/>
-    <col min="11" max="11" width="21.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7142857142857" style="1" customWidth="1"/>
-    <col min="13" max="14" width="17.8380952380952" style="12" customWidth="1"/>
-    <col min="15" max="37" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="38" max="38" width="17.8380952380952" style="12" customWidth="1"/>
-    <col min="39" max="39" width="35.5714285714286" style="1" customWidth="1"/>
-    <col min="40" max="40" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="41" max="41" width="20.8571428571429" style="1" customWidth="1"/>
-    <col min="42" max="42" width="9.14285714285714" style="1"/>
-    <col min="43" max="43" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="44" max="44" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="45" max="45" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="46" max="16384" width="9.14285714285714" style="1"/>
+    <col min="6" max="6" width="22.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.859375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.8359375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="21.4296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="17.8359375" style="10" customWidth="1"/>
+    <col min="15" max="37" width="17.8359375" style="1" customWidth="1"/>
+    <col min="38" max="38" width="17.8359375" style="10" customWidth="1"/>
+    <col min="39" max="39" width="35.5703125" style="1" customWidth="1"/>
+    <col min="40" max="40" width="15.2890625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="20.859375" style="1" customWidth="1"/>
+    <col min="42" max="42" width="9.140625" style="1"/>
+    <col min="43" max="43" width="15.5703125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="17.7109375" style="1" customWidth="1"/>
+    <col min="45" max="45" width="17.4296875" style="1" customWidth="1"/>
+    <col min="46" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:41">
@@ -1914,106 +1908,106 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="T1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="U1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="W1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="X1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Y1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="Z1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AA1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AB1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="22" t="s">
+      <c r="AC1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="23" t="s">
+      <c r="AD1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="23" t="s">
+      <c r="AE1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="22" t="s">
+      <c r="AF1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="22" t="s">
+      <c r="AG1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="23" t="s">
+      <c r="AH1" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="23" t="s">
+      <c r="AI1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="18" t="s">
+      <c r="AJ1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="18" t="s">
+      <c r="AK1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="18" t="s">
+      <c r="AL1" s="16" t="s">
         <v>37</v>
       </c>
       <c r="AM1" s="8" t="s">
@@ -2027,1278 +2021,1262 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:41">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20" t="s">
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK2" s="25" t="s">
+      <c r="AK2" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AL2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AM2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN2" s="10">
+      <c r="AN2" s="7">
         <v>200</v>
       </c>
-      <c r="AO2" s="20" t="s">
+      <c r="AO2" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:41">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
-      <c r="AH3" s="20"/>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="20" t="s">
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="18"/>
+      <c r="AH3" s="18"/>
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK3" s="25" t="s">
+      <c r="AK3" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="20" t="s">
+      <c r="AL3" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM3" s="5" t="s">
+      <c r="AM3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN3" s="10">
+      <c r="AN3" s="7">
         <v>200</v>
       </c>
-      <c r="AO3" s="20" t="s">
+      <c r="AO3" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:41">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
-      <c r="AH4" s="20"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="20" t="s">
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK4" s="25" t="s">
+      <c r="AK4" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL4" s="20" t="s">
+      <c r="AL4" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM4" s="5" t="s">
+      <c r="AM4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN4" s="10">
+      <c r="AN4" s="7">
         <v>200</v>
       </c>
-      <c r="AO4" s="20" t="s">
+      <c r="AO4" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:41">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="20"/>
-      <c r="AD5" s="20"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="20"/>
-      <c r="AI5" s="20"/>
-      <c r="AJ5" s="20" t="s">
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK5" s="25" t="s">
+      <c r="AK5" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL5" s="20" t="s">
+      <c r="AL5" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM5" s="5" t="s">
+      <c r="AM5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN5" s="10">
+      <c r="AN5" s="7">
         <v>200</v>
       </c>
-      <c r="AO5" s="20" t="s">
+      <c r="AO5" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" customHeight="1" spans="1:41">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="20" t="s">
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="24" t="s">
+      <c r="M6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P6" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q6" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="R6" s="20" t="s">
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="S6" s="20" t="s">
+      <c r="S6" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="T6" s="24" t="s">
+      <c r="T6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="U6" s="24" t="s">
+      <c r="U6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="V6" s="10" t="s">
+      <c r="V6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="24" t="s">
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z6" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="X6" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y6" s="20" t="s">
+      <c r="AA6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="Z6" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA6" s="24" t="s">
+      <c r="AG6" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AB6" s="24" t="s">
+      <c r="AI6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AC6" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD6" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE6" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF6" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG6" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH6" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI6" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ6" s="20" t="s">
+      <c r="AJ6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK6" s="25" t="s">
+      <c r="AK6" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL6" s="20" t="s">
+      <c r="AL6" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM6" s="5" t="s">
+      <c r="AM6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN6" s="10">
+      <c r="AN6" s="7">
         <v>200</v>
       </c>
-      <c r="AO6" s="20" t="s">
+      <c r="AO6" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:41">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="24" t="s">
+      <c r="M7" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N7" s="24" t="s">
+      <c r="N7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="Q7" s="24" t="s">
+      <c r="Q7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="R7" s="20" t="s">
+      <c r="R7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="20" t="s">
+      <c r="S7" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="T7" s="24" t="s">
+      <c r="T7" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="U7" s="24" t="s">
+      <c r="U7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="V7" s="10" t="s">
+      <c r="V7" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="W7" s="24" t="s">
+      <c r="W7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="X7" s="24" t="s">
+      <c r="X7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="Y7" s="20" t="s">
+      <c r="Y7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="Z7" s="20" t="s">
+      <c r="Z7" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA7" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC7" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AA7" s="24" t="s">
+      <c r="AD7" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE7" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG7" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH7" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AB7" s="24" t="s">
+      <c r="AI7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AC7" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD7" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE7" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF7" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG7" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH7" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI7" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ7" s="20" t="s">
+      <c r="AJ7" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK7" s="25" t="s">
+      <c r="AK7" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL7" s="20" t="s">
+      <c r="AL7" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM7" s="5" t="s">
+      <c r="AM7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN7" s="10">
+      <c r="AN7" s="7">
         <v>200</v>
       </c>
-      <c r="AO7" s="20" t="s">
+      <c r="AO7" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:41">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="24" t="s">
+      <c r="M8" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="N8" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="Q8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="R8" s="20" t="s">
+      <c r="R8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="S8" s="20" t="s">
+      <c r="S8" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="T8" s="24" t="s">
+      <c r="T8" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="U8" s="24" t="s">
+      <c r="U8" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="V8" s="10" t="s">
+      <c r="V8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="W8" s="24" t="s">
+      <c r="W8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="X8" s="24" t="s">
+      <c r="X8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="Y8" s="20" t="s">
+      <c r="Y8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="Z8" s="20" t="s">
+      <c r="Z8" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA8" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB8" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AA8" s="24" t="s">
+      <c r="AD8" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE8" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG8" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH8" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AB8" s="24" t="s">
+      <c r="AI8" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AC8" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD8" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE8" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF8" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG8" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH8" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI8" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ8" s="20" t="s">
+      <c r="AJ8" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK8" s="25" t="s">
+      <c r="AK8" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL8" s="20" t="s">
+      <c r="AL8" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM8" s="5" t="s">
+      <c r="AM8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN8" s="10">
+      <c r="AN8" s="7">
         <v>200</v>
       </c>
-      <c r="AO8" s="20" t="s">
+      <c r="AO8" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:41">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="L9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M9" s="24" t="s">
+      <c r="M9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="24" t="s">
+      <c r="N9" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="O9" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="P9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="Q9" s="24" t="s">
+      <c r="Q9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="R9" s="20" t="s">
+      <c r="R9" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="S9" s="20" t="s">
+      <c r="S9" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="T9" s="24" t="s">
+      <c r="T9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="24" t="s">
+      <c r="U9" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="V9" s="10" t="s">
+      <c r="V9" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="W9" s="24" t="s">
+      <c r="W9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="X9" s="24" t="s">
+      <c r="X9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="Y9" s="20" t="s">
+      <c r="Y9" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="Z9" s="20" t="s">
+      <c r="Z9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA9" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB9" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC9" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AA9" s="24" t="s">
+      <c r="AD9" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE9" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG9" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AB9" s="24" t="s">
+      <c r="AI9" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AC9" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD9" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE9" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF9" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG9" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH9" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI9" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ9" s="20" t="s">
+      <c r="AJ9" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK9" s="25" t="s">
+      <c r="AK9" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL9" s="20" t="s">
+      <c r="AL9" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM9" s="5" t="s">
+      <c r="AM9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN9" s="10">
+      <c r="AN9" s="7">
         <v>200</v>
       </c>
-      <c r="AO9" s="20" t="s">
+      <c r="AO9" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" customHeight="1" spans="1:41">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="S10" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="V10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="W10" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="M10" s="24" t="s">
+      <c r="X10" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y10" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z10" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA10" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="AB10" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="O10" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="P10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="S10" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="T10" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="U10" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="V10" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="W10" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="X10" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y10" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z10" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA10" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB10" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="24"/>
-      <c r="AE10" s="24"/>
-      <c r="AF10" s="20"/>
-      <c r="AG10" s="20"/>
-      <c r="AH10" s="24"/>
-      <c r="AI10" s="24"/>
-      <c r="AJ10" s="20" t="s">
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="18"/>
+      <c r="AG10" s="18"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK10" s="25" t="s">
+      <c r="AK10" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL10" s="20" t="s">
+      <c r="AL10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM10" s="5" t="s">
+      <c r="AM10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN10" s="10">
+      <c r="AN10" s="7">
         <v>200</v>
       </c>
-      <c r="AO10" s="20" t="s">
+      <c r="AO10" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:41">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="D11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="S11" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="T11" s="24" t="s">
+      <c r="T11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="U11" s="24" t="s">
+      <c r="U11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="V11" s="10" t="s">
+      <c r="V11" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="W11" s="24" t="s">
+      <c r="W11" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="X11" s="24" t="s">
+      <c r="X11" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="Y11" s="20" t="s">
+      <c r="Y11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="Z11" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA11" s="24" t="s">
+      <c r="Z11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AB11" s="24" t="s">
+      <c r="AB11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AC11" s="10"/>
-      <c r="AD11" s="24"/>
-      <c r="AE11" s="24"/>
-      <c r="AF11" s="20"/>
-      <c r="AG11" s="20"/>
-      <c r="AH11" s="24"/>
-      <c r="AI11" s="24"/>
-      <c r="AJ11" s="20" t="s">
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="18"/>
+      <c r="AG11" s="18"/>
+      <c r="AH11" s="20"/>
+      <c r="AI11" s="20"/>
+      <c r="AJ11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK11" s="25" t="s">
+      <c r="AK11" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL11" s="20" t="s">
+      <c r="AL11" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM11" s="5" t="s">
+      <c r="AM11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN11" s="10">
+      <c r="AN11" s="7">
         <v>200</v>
       </c>
-      <c r="AO11" s="20" t="s">
+      <c r="AO11" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:41">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="20" t="s">
+      <c r="D12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="20" t="s">
+      <c r="L12" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="M12" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="O12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P12" s="24" t="s">
+      <c r="P12" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="Q12" s="24" t="s">
+      <c r="Q12" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="R12" s="20" t="s">
+      <c r="R12" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="S12" s="20" t="s">
+      <c r="S12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="T12" s="24" t="s">
+      <c r="T12" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="U12" s="24" t="s">
+      <c r="U12" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="V12" s="10" t="s">
+      <c r="V12" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="W12" s="24" t="s">
+      <c r="W12" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="X12" s="24" t="s">
+      <c r="X12" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="Y12" s="20" t="s">
+      <c r="Y12" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="Z12" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA12" s="24" t="s">
+      <c r="Z12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA12" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AB12" s="24" t="s">
+      <c r="AB12" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AC12" s="10"/>
-      <c r="AD12" s="24"/>
-      <c r="AE12" s="24"/>
-      <c r="AF12" s="20"/>
-      <c r="AG12" s="20"/>
-      <c r="AH12" s="24"/>
-      <c r="AI12" s="24"/>
-      <c r="AJ12" s="20" t="s">
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="18"/>
+      <c r="AG12" s="18"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK12" s="25" t="s">
+      <c r="AK12" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL12" s="20" t="s">
+      <c r="AL12" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM12" s="5" t="s">
+      <c r="AM12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN12" s="10">
+      <c r="AN12" s="7">
         <v>200</v>
       </c>
-      <c r="AO12" s="20" t="s">
+      <c r="AO12" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:41">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="20" t="s">
+      <c r="D13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="K13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="L13" s="20" t="s">
+      <c r="L13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="M13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N13" s="24" t="s">
+      <c r="N13" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O13" s="10" t="s">
+      <c r="O13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P13" s="24" t="s">
+      <c r="P13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="Q13" s="24" t="s">
+      <c r="Q13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="S13" s="20" t="s">
+      <c r="S13" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="T13" s="24" t="s">
+      <c r="T13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="U13" s="24" t="s">
+      <c r="U13" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="V13" s="10" t="s">
+      <c r="V13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="W13" s="24" t="s">
+      <c r="W13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="X13" s="24" t="s">
+      <c r="X13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="Y13" s="20" t="s">
+      <c r="Y13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="Z13" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA13" s="24" t="s">
+      <c r="Z13" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AB13" s="24" t="s">
+      <c r="AB13" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AC13" s="10"/>
-      <c r="AD13" s="24"/>
-      <c r="AE13" s="24"/>
-      <c r="AF13" s="20"/>
-      <c r="AG13" s="20"/>
-      <c r="AH13" s="24"/>
-      <c r="AI13" s="24"/>
-      <c r="AJ13" s="20" t="s">
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="18"/>
+      <c r="AG13" s="18"/>
+      <c r="AH13" s="20"/>
+      <c r="AI13" s="20"/>
+      <c r="AJ13" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK13" s="25" t="s">
+      <c r="AK13" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AL13" s="20" t="s">
+      <c r="AL13" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AM13" s="5" t="s">
+      <c r="AM13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN13" s="10">
+      <c r="AN13" s="7">
         <v>200</v>
       </c>
-      <c r="AO13" s="20" t="s">
+      <c r="AO13" s="18" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3317,20 +3295,20 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.2857142857143" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.2857142857143" style="12" customWidth="1"/>
-    <col min="10" max="10" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="20.2890625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.2890625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.2890625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.4296875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:9">
@@ -3346,10 +3324,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>105</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -3363,31 +3341,31 @@
       </c>
     </row>
     <row r="2" ht="59" customHeight="1" spans="1:9">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>200</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3406,24 +3384,24 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="33.7142857142857" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.8571428571429" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="12" customWidth="1"/>
-    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.2857142857143" style="12" customWidth="1"/>
-    <col min="12" max="12" width="20.5714285714286" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="24.859375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="31.4296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2890625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2890625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4296875" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
@@ -3439,16 +3417,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>128</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -3457,52 +3435,52 @@
       <c r="J1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="7">
         <v>200</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3521,24 +3499,24 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="33.7142857142857" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.8571428571429" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="12" customWidth="1"/>
-    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.2857142857143" style="12" customWidth="1"/>
-    <col min="12" max="12" width="20.5714285714286" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="24.859375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="31.4296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2890625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2890625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4296875" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
@@ -3554,16 +3532,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>128</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -3572,52 +3550,52 @@
       <c r="J1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="7">
         <v>200</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3636,24 +3614,24 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="33.7142857142857" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.8571428571429" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="12" customWidth="1"/>
-    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.2857142857143" style="12" customWidth="1"/>
-    <col min="12" max="12" width="20.5714285714286" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="24.859375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="31.4296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2890625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2890625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4296875" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
@@ -3669,16 +3647,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>128</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -3687,52 +3665,52 @@
       <c r="J1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="7">
         <v>200</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3751,24 +3729,24 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="33.7142857142857" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.8571428571429" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="12" customWidth="1"/>
-    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.2857142857143" style="12" customWidth="1"/>
-    <col min="12" max="12" width="20.5714285714286" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="24.859375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="31.4296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2890625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2890625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4296875" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
@@ -3784,16 +3762,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>128</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -3802,52 +3780,52 @@
       <c r="J1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="7">
         <v>200</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3866,24 +3844,24 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="26.5714285714286" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.4285714285714" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.4296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
-    <col min="9" max="10" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.2857142857143" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.14285714285714" style="1"/>
-    <col min="14" max="14" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="31.4296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.2890625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.2890625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.4296875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:12">
@@ -3899,19 +3877,19 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="8" t="s">
@@ -3925,40 +3903,40 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:12">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3973,29 +3951,29 @@
   <sheetPr/>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="26.5714285714286" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.4285714285714" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.4296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.2857142857143" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5714285714286" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5714285714286" style="1" customWidth="1"/>
-    <col min="9" max="9" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.2857142857143" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1428571428571" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.2857142857143" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="30.2890625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.2890625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="31.4296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.2890625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.2890625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.2890625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.4296875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:16">
@@ -4011,16 +3989,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>155</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -4049,16 +4027,16 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="84" customHeight="1" spans="1:16">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>163</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -4073,42 +4051,42 @@
       <c r="H2" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="7">
         <v>200</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="7">
         <v>2</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="7">
         <v>2</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="7">
         <v>1</v>
       </c>
-      <c r="P2" s="10">
+      <c r="P2" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="84" customHeight="1" spans="1:16">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>163</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -4123,42 +4101,42 @@
       <c r="H3" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="7">
         <v>200</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="7">
         <v>2</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="7">
         <v>2</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="7">
         <v>1</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="84" customHeight="1" spans="1:16">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>163</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -4173,42 +4151,42 @@
       <c r="H4" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="7">
         <v>200</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="7">
         <v>2</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="7">
         <v>2</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="7">
         <v>1</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="84" customHeight="1" spans="1:16">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>163</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -4223,28 +4201,28 @@
       <c r="H5" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="7">
         <v>200</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="7">
         <v>2</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="7">
         <v>2</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="7">
         <v>1</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="7">
         <v>2</v>
       </c>
     </row>
@@ -4263,25 +4241,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7142857142857" style="1" customWidth="1"/>
-    <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.2857142857143" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.14285714285714" style="1"/>
-    <col min="14" max="14" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.4296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.2890625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.2890625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.4296875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:12">
@@ -4297,19 +4275,19 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="6" t="s">
         <v>97</v>
       </c>
       <c r="J1" s="8" t="s">
@@ -4323,40 +4301,40 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:12">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="7">
         <v>18</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="7">
         <v>18</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>18</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4375,25 +4353,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
-    <col min="9" max="12" width="19.7142857142857" style="1" customWidth="1"/>
-    <col min="13" max="13" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.2857142857143" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.14285714285714" style="1"/>
-    <col min="17" max="17" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.4296875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.2890625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.2890625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="15.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.4296875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
@@ -4409,28 +4387,28 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="6" t="s">
         <v>97</v>
       </c>
       <c r="M1" s="8" t="s">
@@ -4444,45 +4422,45 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="7">
         <v>18</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>18</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="7">
         <v>18</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="10" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="7">
         <v>200</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4501,25 +4479,25 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
-    <col min="9" max="12" width="19.7142857142857" style="1" customWidth="1"/>
-    <col min="13" max="13" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.2857142857143" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.14285714285714" style="1"/>
-    <col min="17" max="17" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.4296875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.2890625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.2890625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="15.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.4296875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
@@ -4535,28 +4513,28 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="6" t="s">
         <v>97</v>
       </c>
       <c r="M1" s="8" t="s">
@@ -4570,45 +4548,45 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="7">
         <v>18</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>18</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="7">
         <v>18</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="10" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="7">
         <v>200</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4627,25 +4605,25 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
-    <col min="9" max="12" width="19.7142857142857" style="1" customWidth="1"/>
-    <col min="13" max="13" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.2857142857143" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.14285714285714" style="1"/>
-    <col min="17" max="17" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.4296875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.2890625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.2890625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="15.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.4296875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
@@ -4661,28 +4639,28 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="6" t="s">
         <v>97</v>
       </c>
       <c r="M1" s="8" t="s">
@@ -4696,45 +4674,45 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="7">
         <v>18</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>18</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="7">
         <v>18</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="10" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="7">
         <v>200</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4753,25 +4731,25 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5714285714286" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="1" customWidth="1"/>
-    <col min="9" max="12" width="19.7142857142857" style="1" customWidth="1"/>
-    <col min="13" max="13" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.2857142857143" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.14285714285714" style="1"/>
-    <col min="17" max="17" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2890625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.4296875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.2890625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.2890625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="15.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.4296875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
@@ -4787,28 +4765,28 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="6" t="s">
         <v>97</v>
       </c>
       <c r="M1" s="8" t="s">
@@ -4822,45 +4800,45 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="10">
+      <c r="F2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="7">
         <v>18</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>18</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="7">
         <v>18</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="10" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="7">
         <v>200</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4879,20 +4857,20 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="34.5714285714286" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.2857142857143" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.2857142857143" style="12" customWidth="1"/>
-    <col min="10" max="10" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="20.2890625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.2890625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.2890625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.4296875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:9">
@@ -4908,10 +4886,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>105</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -4925,31 +4903,31 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="59" customHeight="1" spans="1:9">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>200</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4968,20 +4946,20 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="36.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.2857142857143" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.2857142857143" style="12" customWidth="1"/>
-    <col min="10" max="10" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="20.2890625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.2890625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.2890625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.4296875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:9">
@@ -4997,10 +4975,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>105</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -5014,31 +4992,31 @@
       </c>
     </row>
     <row r="2" ht="59" customHeight="1" spans="1:9">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>200</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5057,20 +5035,20 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="41" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.2857142857143" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.2857142857143" style="12" customWidth="1"/>
-    <col min="10" max="10" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="5" width="20.2890625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.4296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.2890625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.2890625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.4296875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:9">
@@ -5086,10 +5064,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>105</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -5103,31 +5081,31 @@
       </c>
     </row>
     <row r="2" ht="59" customHeight="1" spans="1:9">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>200</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
flow agent and restaurannt
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/GO_Course_Information.xlsx
+++ b/src/main/resources/input_excel_file/booking/GO_Course_Information.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="6" activeTab="10"/>
+    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Create_Flight" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Delete_Attach_Flight_Player3" sheetId="14" r:id="rId13"/>
     <sheet name="Delete_Attach_Flight_Player4" sheetId="15" r:id="rId14"/>
     <sheet name="Add_Bag_To_Flight" sheetId="6" r:id="rId15"/>
-    <sheet name="Add_Round" sheetId="16" r:id="rId16"/>
+    <sheet name="Add_Round_Player1" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3376,7 +3376,7 @@
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -3947,8 +3947,8 @@
   <sheetPr/>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="4"/>
@@ -4346,7 +4346,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>

</xml_diff>